<commit_message>
Commit new file CDA2 LAB
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/Medica/3.2.0.0/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/Medica/3.2.0.0/accreditamento-checklist_V8.1.3.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="516">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -204,7 +204,7 @@
     <t xml:space="preserve">NOME FORNITORE:</t>
   </si>
   <si>
-    <t xml:space="preserve">Multimedia Srl</t>
+    <t xml:space="preserve">Multimedia srl</t>
   </si>
   <si>
     <t xml:space="preserve">IDENTIFICATIVI SOFTWARE</t>
@@ -435,13 +435,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-21T07:08:11Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f75e81ef25fad9f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.8f7e930e354d782a9f9d1193ec7d3ccf3760dff2a3e9bb659f30fe0c765fd0e2.7c7a3d21a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-24T12:56:13Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">462375c5ace95b81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.dcbac99ecb790313e84ce73b73c3723abfd5d41c43e82fe108c955073c408e4b.828321fd81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">LDO</t>
@@ -1527,9 +1527,6 @@
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-44| Il codice fiscale 'PzNMSC00A01F839U' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’errore è registrato in un log applicativo; l’operatore può provare a correggere l’errore e generare un nuovo referto oppure firmare il referto contenente il CDA2 non validato. </t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RSA_CT7_KO</t>
@@ -2549,10 +2546,10 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2635,11 +2632,11 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -2667,7 +2664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
@@ -2683,7 +2680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
@@ -2715,7 +2712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="n">
         <v>8</v>
       </c>
@@ -2723,7 +2720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
         <v>9</v>
       </c>
@@ -2731,7 +2728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
         <v>10</v>
       </c>
@@ -2752,7 +2749,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:T1048576"/>
@@ -2762,10 +2759,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J56" activeCellId="0" sqref="J56"/>
+      <selection pane="bottomRight" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -3015,7 +3012,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="n">
         <v>1</v>
       </c>
@@ -3059,7 +3056,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="n">
         <v>2</v>
       </c>
@@ -3103,7 +3100,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="24" t="n">
         <v>3</v>
       </c>
@@ -3147,7 +3144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="n">
         <v>4</v>
       </c>
@@ -3191,7 +3188,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="n">
         <v>5</v>
       </c>
@@ -3208,7 +3205,7 @@
         <v>73</v>
       </c>
       <c r="F14" s="27" t="n">
-        <v>45128</v>
+        <v>45131</v>
       </c>
       <c r="G14" s="28" t="s">
         <v>74</v>
@@ -3279,7 +3276,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="n">
         <v>7</v>
       </c>
@@ -3317,7 +3314,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="n">
         <v>8</v>
       </c>
@@ -3355,7 +3352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="n">
         <v>9</v>
       </c>
@@ -3393,7 +3390,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="n">
         <v>11</v>
       </c>
@@ -3437,7 +3434,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="n">
         <v>12</v>
       </c>
@@ -3475,7 +3472,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="n">
         <v>13</v>
       </c>
@@ -3513,7 +3510,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="n">
         <v>14</v>
       </c>
@@ -3551,7 +3548,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="n">
         <v>28</v>
       </c>
@@ -3593,7 +3590,7 @@
         <v>108</v>
       </c>
       <c r="O23" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P23" s="29" t="s">
         <v>109</v>
@@ -3605,7 +3602,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="100.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="n">
         <v>29</v>
       </c>
@@ -3647,7 +3644,7 @@
         <v>108</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P24" s="29" t="s">
         <v>109</v>
@@ -3659,7 +3656,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="100.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="n">
         <v>31</v>
       </c>
@@ -3701,7 +3698,7 @@
         <v>108</v>
       </c>
       <c r="O25" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P25" s="29" t="s">
         <v>109</v>
@@ -3713,7 +3710,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="100.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="n">
         <v>32</v>
       </c>
@@ -3755,7 +3752,7 @@
         <v>121</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P26" s="29" t="s">
         <v>109</v>
@@ -3767,7 +3764,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="n">
         <v>36</v>
       </c>
@@ -3809,7 +3806,7 @@
         <v>126</v>
       </c>
       <c r="O27" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P27" s="29" t="s">
         <v>109</v>
@@ -3821,7 +3818,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="100.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="n">
         <v>37</v>
       </c>
@@ -3863,7 +3860,7 @@
         <v>126</v>
       </c>
       <c r="O28" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P28" s="29" t="s">
         <v>109</v>
@@ -3875,7 +3872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="100.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="n">
         <v>39</v>
       </c>
@@ -3917,7 +3914,7 @@
         <v>126</v>
       </c>
       <c r="O29" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P29" s="29" t="s">
         <v>109</v>
@@ -3929,7 +3926,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="100.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="n">
         <v>40</v>
       </c>
@@ -3971,7 +3968,7 @@
         <v>126</v>
       </c>
       <c r="O30" s="29" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="P30" s="29" t="s">
         <v>109</v>
@@ -3983,7 +3980,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="n">
         <v>44</v>
       </c>
@@ -4031,7 +4028,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="n">
         <v>45</v>
       </c>
@@ -4079,7 +4076,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="n">
         <v>47</v>
       </c>
@@ -4127,7 +4124,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="24" t="n">
         <v>48</v>
       </c>
@@ -4175,7 +4172,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="24" t="n">
         <v>52</v>
       </c>
@@ -4229,7 +4226,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="24" t="n">
         <v>53</v>
       </c>
@@ -4283,7 +4280,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="24" t="n">
         <v>54</v>
       </c>
@@ -4337,7 +4334,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="n">
         <v>55</v>
       </c>
@@ -4391,7 +4388,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="24" t="n">
         <v>56</v>
       </c>
@@ -4445,7 +4442,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="24" t="n">
         <v>57</v>
       </c>
@@ -4499,7 +4496,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="24" t="n">
         <v>58</v>
       </c>
@@ -4553,7 +4550,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="24" t="n">
         <v>59</v>
       </c>
@@ -4607,7 +4604,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="348.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="24" t="n">
         <v>60</v>
       </c>
@@ -4661,7 +4658,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="24" t="n">
         <v>61</v>
       </c>
@@ -4715,7 +4712,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="236.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="24" t="n">
         <v>62</v>
       </c>
@@ -5201,7 +5198,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="24" t="n">
         <v>71</v>
       </c>
@@ -5239,7 +5236,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="24" t="n">
         <v>72</v>
       </c>
@@ -5331,7 +5328,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="24" t="n">
         <v>74</v>
       </c>
@@ -5369,7 +5366,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="24" t="n">
         <v>75</v>
       </c>
@@ -5410,8 +5407,12 @@
       <c r="N58" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="O58" s="29"/>
-      <c r="P58" s="29"/>
+      <c r="O58" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P58" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q58" s="29"/>
       <c r="R58" s="30"/>
       <c r="S58" s="31"/>
@@ -5419,7 +5420,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="24" t="n">
         <v>76</v>
       </c>
@@ -5460,8 +5461,12 @@
       <c r="N59" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="O59" s="29"/>
-      <c r="P59" s="29"/>
+      <c r="O59" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P59" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q59" s="29"/>
       <c r="R59" s="30"/>
       <c r="S59" s="31"/>
@@ -5469,7 +5474,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="24" t="n">
         <v>77</v>
       </c>
@@ -5510,8 +5515,12 @@
       <c r="N60" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="O60" s="29"/>
-      <c r="P60" s="29"/>
+      <c r="O60" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P60" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q60" s="29"/>
       <c r="R60" s="30"/>
       <c r="S60" s="31"/>
@@ -5519,7 +5528,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="24" t="n">
         <v>78</v>
       </c>
@@ -5560,8 +5569,12 @@
       <c r="N61" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="O61" s="29"/>
-      <c r="P61" s="29"/>
+      <c r="O61" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P61" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q61" s="29"/>
       <c r="R61" s="30"/>
       <c r="S61" s="31"/>
@@ -5569,7 +5582,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="24" t="n">
         <v>79</v>
       </c>
@@ -5610,8 +5623,12 @@
       <c r="N62" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="O62" s="29"/>
-      <c r="P62" s="29"/>
+      <c r="O62" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P62" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q62" s="29"/>
       <c r="R62" s="30"/>
       <c r="S62" s="31"/>
@@ -5619,7 +5636,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="24" t="n">
         <v>80</v>
       </c>
@@ -5660,8 +5677,12 @@
       <c r="N63" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="O63" s="29"/>
-      <c r="P63" s="29"/>
+      <c r="O63" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P63" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q63" s="29"/>
       <c r="R63" s="30"/>
       <c r="S63" s="31"/>
@@ -5669,7 +5690,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="24" t="n">
         <v>81</v>
       </c>
@@ -5707,7 +5728,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="24" t="n">
         <v>82</v>
       </c>
@@ -5748,8 +5769,12 @@
       <c r="N65" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="O65" s="29"/>
-      <c r="P65" s="29"/>
+      <c r="O65" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P65" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q65" s="29"/>
       <c r="R65" s="30"/>
       <c r="S65" s="31"/>
@@ -5757,7 +5782,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="24" t="n">
         <v>83</v>
       </c>
@@ -5798,8 +5823,12 @@
       <c r="N66" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="O66" s="29"/>
-      <c r="P66" s="29"/>
+      <c r="O66" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P66" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q66" s="29"/>
       <c r="R66" s="30"/>
       <c r="S66" s="31"/>
@@ -5807,7 +5836,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="24" t="n">
         <v>84</v>
       </c>
@@ -5848,8 +5877,12 @@
       <c r="N67" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="O67" s="29"/>
-      <c r="P67" s="29"/>
+      <c r="O67" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P67" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q67" s="29"/>
       <c r="R67" s="30"/>
       <c r="S67" s="31"/>
@@ -5857,7 +5890,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="24" t="n">
         <v>85</v>
       </c>
@@ -5898,8 +5931,12 @@
       <c r="N68" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="O68" s="29"/>
-      <c r="P68" s="29"/>
+      <c r="O68" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P68" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q68" s="29"/>
       <c r="R68" s="30"/>
       <c r="S68" s="31"/>
@@ -5907,7 +5944,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="24" t="n">
         <v>86</v>
       </c>
@@ -5945,7 +5982,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="24" t="n">
         <v>87</v>
       </c>
@@ -5983,7 +6020,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="24" t="n">
         <v>88</v>
       </c>
@@ -6021,7 +6058,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="24" t="n">
         <v>89</v>
       </c>
@@ -6059,7 +6096,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="24" t="n">
         <v>90</v>
       </c>
@@ -6097,7 +6134,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="24" t="n">
         <v>91</v>
       </c>
@@ -6135,7 +6172,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="24" t="n">
         <v>92</v>
       </c>
@@ -6173,7 +6210,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="24" t="n">
         <v>93</v>
       </c>
@@ -6214,8 +6251,12 @@
       <c r="N76" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="O76" s="29"/>
-      <c r="P76" s="29"/>
+      <c r="O76" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="P76" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="Q76" s="29"/>
       <c r="R76" s="30"/>
       <c r="S76" s="31"/>
@@ -6223,7 +6264,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="24" t="n">
         <v>147</v>
       </c>
@@ -6267,7 +6308,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="24" t="n">
         <v>148</v>
       </c>
@@ -6305,7 +6346,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="24" t="n">
         <v>149</v>
       </c>
@@ -6343,7 +6384,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="24" t="n">
         <v>150</v>
       </c>
@@ -6381,7 +6422,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="24" t="n">
         <v>151</v>
       </c>
@@ -6435,7 +6476,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="24" t="n">
         <v>152</v>
       </c>
@@ -6480,7 +6521,7 @@
         <v>85</v>
       </c>
       <c r="P82" s="29" t="s">
-        <v>368</v>
+        <v>148</v>
       </c>
       <c r="Q82" s="29"/>
       <c r="R82" s="30"/>
@@ -6489,7 +6530,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="89.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="24" t="n">
         <v>153</v>
       </c>
@@ -6500,22 +6541,22 @@
         <v>117</v>
       </c>
       <c r="D83" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="E83" s="26" t="s">
         <v>369</v>
-      </c>
-      <c r="E83" s="26" t="s">
-        <v>370</v>
       </c>
       <c r="F83" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G83" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="H83" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="H83" s="28" t="s">
+      <c r="I83" s="28" t="s">
         <v>372</v>
-      </c>
-      <c r="I83" s="28" t="s">
-        <v>373</v>
       </c>
       <c r="J83" s="29" t="s">
         <v>55</v>
@@ -6528,7 +6569,7 @@
         <v>55</v>
       </c>
       <c r="N83" s="29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O83" s="29" t="s">
         <v>85</v>
@@ -6543,7 +6584,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="89.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="24" t="n">
         <v>154</v>
       </c>
@@ -6554,22 +6595,22 @@
         <v>117</v>
       </c>
       <c r="D84" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="E84" s="26" t="s">
         <v>375</v>
-      </c>
-      <c r="E84" s="26" t="s">
-        <v>376</v>
       </c>
       <c r="F84" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G84" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="H84" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="H84" s="28" t="s">
+      <c r="I84" s="28" t="s">
         <v>378</v>
-      </c>
-      <c r="I84" s="28" t="s">
-        <v>379</v>
       </c>
       <c r="J84" s="29" t="s">
         <v>55</v>
@@ -6597,7 +6638,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="24" t="n">
         <v>155</v>
       </c>
@@ -6608,22 +6649,22 @@
         <v>117</v>
       </c>
       <c r="D85" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="E85" s="26" t="s">
         <v>380</v>
-      </c>
-      <c r="E85" s="26" t="s">
-        <v>381</v>
       </c>
       <c r="F85" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G85" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="H85" s="28" t="s">
         <v>382</v>
       </c>
-      <c r="H85" s="28" t="s">
+      <c r="I85" s="28" t="s">
         <v>383</v>
-      </c>
-      <c r="I85" s="28" t="s">
-        <v>384</v>
       </c>
       <c r="J85" s="29" t="s">
         <v>55</v>
@@ -6651,7 +6692,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="24" t="n">
         <v>156</v>
       </c>
@@ -6662,22 +6703,22 @@
         <v>117</v>
       </c>
       <c r="D86" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="E86" s="26" t="s">
         <v>385</v>
-      </c>
-      <c r="E86" s="26" t="s">
-        <v>386</v>
       </c>
       <c r="F86" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G86" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="H86" s="28" t="s">
         <v>387</v>
       </c>
-      <c r="H86" s="28" t="s">
+      <c r="I86" s="28" t="s">
         <v>388</v>
-      </c>
-      <c r="I86" s="28" t="s">
-        <v>389</v>
       </c>
       <c r="J86" s="29" t="s">
         <v>55</v>
@@ -6705,7 +6746,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="24" t="n">
         <v>157</v>
       </c>
@@ -6716,22 +6757,22 @@
         <v>117</v>
       </c>
       <c r="D87" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="E87" s="26" t="s">
         <v>390</v>
-      </c>
-      <c r="E87" s="26" t="s">
-        <v>391</v>
       </c>
       <c r="F87" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G87" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="H87" s="28" t="s">
         <v>392</v>
       </c>
-      <c r="H87" s="28" t="s">
+      <c r="I87" s="28" t="s">
         <v>393</v>
-      </c>
-      <c r="I87" s="28" t="s">
-        <v>394</v>
       </c>
       <c r="J87" s="29" t="s">
         <v>55</v>
@@ -6744,7 +6785,7 @@
         <v>55</v>
       </c>
       <c r="N87" s="29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O87" s="29" t="s">
         <v>85</v>
@@ -6759,7 +6800,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="24" t="n">
         <v>158</v>
       </c>
@@ -6770,22 +6811,22 @@
         <v>117</v>
       </c>
       <c r="D88" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="E88" s="26" t="s">
         <v>396</v>
-      </c>
-      <c r="E88" s="26" t="s">
-        <v>397</v>
       </c>
       <c r="F88" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G88" s="28" t="s">
+        <v>397</v>
+      </c>
+      <c r="H88" s="28" t="s">
         <v>398</v>
       </c>
-      <c r="H88" s="28" t="s">
+      <c r="I88" s="28" t="s">
         <v>399</v>
-      </c>
-      <c r="I88" s="28" t="s">
-        <v>400</v>
       </c>
       <c r="J88" s="29" t="s">
         <v>55</v>
@@ -6798,7 +6839,7 @@
         <v>55</v>
       </c>
       <c r="N88" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O88" s="29" t="s">
         <v>85</v>
@@ -6813,7 +6854,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="24" t="n">
         <v>159</v>
       </c>
@@ -6824,22 +6865,22 @@
         <v>117</v>
       </c>
       <c r="D89" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E89" s="26" t="s">
         <v>402</v>
-      </c>
-      <c r="E89" s="26" t="s">
-        <v>403</v>
       </c>
       <c r="F89" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G89" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="H89" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="H89" s="28" t="s">
+      <c r="I89" s="28" t="s">
         <v>405</v>
-      </c>
-      <c r="I89" s="28" t="s">
-        <v>406</v>
       </c>
       <c r="J89" s="29" t="s">
         <v>55</v>
@@ -6852,7 +6893,7 @@
         <v>55</v>
       </c>
       <c r="N89" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="O89" s="29" t="s">
         <v>85</v>
@@ -6867,7 +6908,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="24" t="n">
         <v>160</v>
       </c>
@@ -6878,22 +6919,22 @@
         <v>117</v>
       </c>
       <c r="D90" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="E90" s="26" t="s">
         <v>408</v>
-      </c>
-      <c r="E90" s="26" t="s">
-        <v>409</v>
       </c>
       <c r="F90" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G90" s="28" t="s">
+        <v>409</v>
+      </c>
+      <c r="H90" s="28" t="s">
         <v>410</v>
       </c>
-      <c r="H90" s="28" t="s">
+      <c r="I90" s="28" t="s">
         <v>411</v>
-      </c>
-      <c r="I90" s="28" t="s">
-        <v>412</v>
       </c>
       <c r="J90" s="29" t="s">
         <v>55</v>
@@ -6906,7 +6947,7 @@
         <v>55</v>
       </c>
       <c r="N90" s="29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="O90" s="29" t="s">
         <v>85</v>
@@ -6921,7 +6962,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="24" t="n">
         <v>161</v>
       </c>
@@ -6932,22 +6973,22 @@
         <v>117</v>
       </c>
       <c r="D91" s="25" t="s">
+        <v>413</v>
+      </c>
+      <c r="E91" s="26" t="s">
         <v>414</v>
-      </c>
-      <c r="E91" s="26" t="s">
-        <v>415</v>
       </c>
       <c r="F91" s="27" t="n">
         <v>45127</v>
       </c>
       <c r="G91" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="H91" s="28" t="s">
         <v>416</v>
       </c>
-      <c r="H91" s="28" t="s">
+      <c r="I91" s="28" t="s">
         <v>417</v>
-      </c>
-      <c r="I91" s="28" t="s">
-        <v>418</v>
       </c>
       <c r="J91" s="29" t="s">
         <v>55</v>
@@ -6960,7 +7001,7 @@
         <v>55</v>
       </c>
       <c r="N91" s="29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="O91" s="29" t="s">
         <v>85</v>
@@ -6975,7 +7016,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="89.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="24" t="n">
         <v>162</v>
       </c>
@@ -6986,10 +7027,10 @@
         <v>117</v>
       </c>
       <c r="D92" s="25" t="s">
+        <v>419</v>
+      </c>
+      <c r="E92" s="26" t="s">
         <v>420</v>
-      </c>
-      <c r="E92" s="26" t="s">
-        <v>421</v>
       </c>
       <c r="F92" s="27"/>
       <c r="G92" s="28"/>
@@ -7013,7 +7054,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="24" t="n">
         <v>163</v>
       </c>
@@ -7024,10 +7065,10 @@
         <v>117</v>
       </c>
       <c r="D93" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="E93" s="26" t="s">
         <v>422</v>
-      </c>
-      <c r="E93" s="26" t="s">
-        <v>423</v>
       </c>
       <c r="F93" s="27"/>
       <c r="G93" s="28"/>
@@ -7051,7 +7092,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="24" t="n">
         <v>164</v>
       </c>
@@ -7062,10 +7103,10 @@
         <v>117</v>
       </c>
       <c r="D94" s="25" t="s">
+        <v>423</v>
+      </c>
+      <c r="E94" s="26" t="s">
         <v>424</v>
-      </c>
-      <c r="E94" s="26" t="s">
-        <v>425</v>
       </c>
       <c r="F94" s="27"/>
       <c r="G94" s="28"/>
@@ -7089,7 +7130,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="24" t="n">
         <v>165</v>
       </c>
@@ -7100,10 +7141,10 @@
         <v>117</v>
       </c>
       <c r="D95" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="E95" s="26" t="s">
         <v>426</v>
-      </c>
-      <c r="E95" s="26" t="s">
-        <v>427</v>
       </c>
       <c r="F95" s="27"/>
       <c r="G95" s="28"/>
@@ -7127,7 +7168,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="24" t="n">
         <v>166</v>
       </c>
@@ -7138,10 +7179,10 @@
         <v>117</v>
       </c>
       <c r="D96" s="25" t="s">
+        <v>427</v>
+      </c>
+      <c r="E96" s="26" t="s">
         <v>428</v>
-      </c>
-      <c r="E96" s="26" t="s">
-        <v>429</v>
       </c>
       <c r="F96" s="27"/>
       <c r="G96" s="28"/>
@@ -7165,7 +7206,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="24" t="n">
         <v>167</v>
       </c>
@@ -7176,10 +7217,10 @@
         <v>117</v>
       </c>
       <c r="D97" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="E97" s="26" t="s">
         <v>430</v>
-      </c>
-      <c r="E97" s="26" t="s">
-        <v>431</v>
       </c>
       <c r="F97" s="27"/>
       <c r="G97" s="28"/>
@@ -7203,7 +7244,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="24" t="n">
         <v>168</v>
       </c>
@@ -7214,10 +7255,10 @@
         <v>117</v>
       </c>
       <c r="D98" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="E98" s="26" t="s">
         <v>432</v>
-      </c>
-      <c r="E98" s="26" t="s">
-        <v>433</v>
       </c>
       <c r="F98" s="27"/>
       <c r="G98" s="28"/>
@@ -7241,7 +7282,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="89.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="24" t="n">
         <v>169</v>
       </c>
@@ -7252,22 +7293,22 @@
         <v>117</v>
       </c>
       <c r="D99" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="E99" s="26" t="s">
         <v>434</v>
-      </c>
-      <c r="E99" s="26" t="s">
-        <v>435</v>
       </c>
       <c r="F99" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G99" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="H99" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="H99" s="28" t="s">
+      <c r="I99" s="28" t="s">
         <v>437</v>
-      </c>
-      <c r="I99" s="28" t="s">
-        <v>438</v>
       </c>
       <c r="J99" s="29" t="s">
         <v>55</v>
@@ -7280,7 +7321,7 @@
         <v>55</v>
       </c>
       <c r="N99" s="29" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="O99" s="29" t="s">
         <v>85</v>
@@ -7295,7 +7336,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="24" t="n">
         <v>368</v>
       </c>
@@ -7306,22 +7347,22 @@
         <v>49</v>
       </c>
       <c r="D100" s="25" t="s">
+        <v>439</v>
+      </c>
+      <c r="E100" s="26" t="s">
         <v>440</v>
-      </c>
-      <c r="E100" s="26" t="s">
-        <v>441</v>
       </c>
       <c r="F100" s="27" t="n">
         <v>45128</v>
       </c>
       <c r="G100" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="H100" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="H100" s="28" t="s">
+      <c r="I100" s="28" t="s">
         <v>443</v>
-      </c>
-      <c r="I100" s="28" t="s">
-        <v>444</v>
       </c>
       <c r="J100" s="29" t="s">
         <v>55</v>
@@ -7350,22 +7391,22 @@
         <v>77</v>
       </c>
       <c r="D101" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="E101" s="26" t="s">
         <v>445</v>
-      </c>
-      <c r="E101" s="26" t="s">
-        <v>446</v>
       </c>
       <c r="F101" s="27" t="n">
         <v>45131</v>
       </c>
       <c r="G101" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="H101" s="28" t="s">
         <v>447</v>
       </c>
-      <c r="H101" s="28" t="s">
+      <c r="I101" s="28" t="s">
         <v>448</v>
-      </c>
-      <c r="I101" s="28" t="s">
-        <v>449</v>
       </c>
       <c r="J101" s="29" t="s">
         <v>55</v>
@@ -7383,7 +7424,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="24" t="n">
         <v>370</v>
       </c>
@@ -7394,22 +7435,22 @@
         <v>91</v>
       </c>
       <c r="D102" s="25" t="s">
+        <v>449</v>
+      </c>
+      <c r="E102" s="26" t="s">
         <v>450</v>
-      </c>
-      <c r="E102" s="26" t="s">
-        <v>451</v>
       </c>
       <c r="F102" s="27" t="n">
         <v>45127</v>
       </c>
       <c r="G102" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="H102" s="28" t="s">
         <v>452</v>
       </c>
-      <c r="H102" s="28" t="s">
+      <c r="I102" s="28" t="s">
         <v>453</v>
-      </c>
-      <c r="I102" s="28" t="s">
-        <v>454</v>
       </c>
       <c r="J102" s="29" t="s">
         <v>55</v>
@@ -7427,7 +7468,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="24" t="n">
         <v>374</v>
       </c>
@@ -7438,22 +7479,22 @@
         <v>117</v>
       </c>
       <c r="D103" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="E103" s="26" t="s">
         <v>455</v>
-      </c>
-      <c r="E103" s="26" t="s">
-        <v>456</v>
       </c>
       <c r="F103" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G103" s="28" t="s">
+        <v>456</v>
+      </c>
+      <c r="H103" s="28" t="s">
         <v>457</v>
       </c>
-      <c r="H103" s="28" t="s">
+      <c r="I103" s="28" t="s">
         <v>458</v>
-      </c>
-      <c r="I103" s="28" t="s">
-        <v>459</v>
       </c>
       <c r="J103" s="29" t="s">
         <v>55</v>
@@ -12403,33 +12444,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A9:T103">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="LDO"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT0"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT1"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT10_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT11_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT12_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT15_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT5_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT6_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT7_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT8_KO"/>
-        <filter val="VALIDAZIONE_CDA2_LDO_CT9_KO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:T103"/>
   <mergeCells count="7">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -12474,7 +12489,7 @@
       <selection pane="bottomLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -12491,10 +12506,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>460</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12502,13 +12517,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>462</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>463</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12516,13 +12531,13 @@
         <v>77</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C3" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>465</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12530,55 +12545,55 @@
         <v>91</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C4" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>467</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="37" t="s">
         <v>469</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="37" t="s">
         <v>470</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>473</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>475</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="C7" s="37" t="s">
+      <c r="D7" s="38" t="s">
         <v>476</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12586,41 +12601,41 @@
         <v>117</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C8" s="37" t="s">
+        <v>477</v>
+      </c>
+      <c r="D8" s="38" t="s">
         <v>478</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C9" s="37" t="s">
         <v>480</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="38" t="s">
         <v>481</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>483</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="C10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>484</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12628,13 +12643,13 @@
         <v>49</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C11" s="37" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12642,13 +12657,13 @@
         <v>77</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C12" s="37" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12656,55 +12671,55 @@
         <v>91</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C13" s="37" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C14" s="37" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C15" s="37" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C16" s="37" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12712,27 +12727,27 @@
         <v>117</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C17" s="37" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C18" s="37" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12740,13 +12755,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C19" s="37" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12754,13 +12769,13 @@
         <v>77</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C20" s="37" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12768,55 +12783,55 @@
         <v>91</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C21" s="37" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C22" s="37" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C23" s="37" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C24" s="37" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12824,27 +12839,27 @@
         <v>117</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C25" s="37" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C26" s="37" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12852,13 +12867,13 @@
         <v>49</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C27" s="37" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12866,13 +12881,13 @@
         <v>77</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C28" s="37" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12880,55 +12895,55 @@
         <v>91</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C29" s="37" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C30" s="37" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C31" s="37" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C32" s="37" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12936,27 +12951,27 @@
         <v>117</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C33" s="37" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C34" s="37" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12964,7 +12979,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C35" s="37" t="n">
         <v>195</v>
@@ -12978,7 +12993,7 @@
         <v>77</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C36" s="37" t="n">
         <v>211</v>
@@ -12992,7 +13007,7 @@
         <v>91</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C37" s="37" t="n">
         <v>227</v>
@@ -13003,10 +13018,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C38" s="37" t="n">
         <v>243</v>
@@ -13017,10 +13032,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C39" s="37" t="n">
         <v>259</v>
@@ -13031,10 +13046,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C40" s="37" t="n">
         <v>275</v>
@@ -13048,7 +13063,7 @@
         <v>117</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C41" s="37" t="n">
         <v>291</v>
@@ -13059,10 +13074,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C42" s="37" t="n">
         <v>307</v>
@@ -13076,7 +13091,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C43" s="37" t="n">
         <v>196</v>
@@ -13090,7 +13105,7 @@
         <v>77</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C44" s="37" t="n">
         <v>212</v>
@@ -13104,7 +13119,7 @@
         <v>91</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C45" s="37" t="n">
         <v>228</v>
@@ -13115,10 +13130,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C46" s="37" t="n">
         <v>244</v>
@@ -13129,10 +13144,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C47" s="37" t="n">
         <v>260</v>
@@ -13143,10 +13158,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C48" s="37" t="n">
         <v>276</v>
@@ -13160,7 +13175,7 @@
         <v>117</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C49" s="37" t="n">
         <v>292</v>
@@ -13171,10 +13186,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C50" s="37" t="n">
         <v>308</v>
@@ -14155,7 +14170,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -14172,7 +14187,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="40" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B2" s="40" t="s">
         <v>55</v>
@@ -14180,7 +14195,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B3" s="40" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
Commit directory with test case and files pdf 2
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/Medica/3.2.0.0/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/Medica/3.2.0.0/accreditamento-checklist_V8.1.3.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="514">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -417,13 +417,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-21T07:05:34Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59f96d640c21e940</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.0efc9b05b695de966137c969b8aadb6d5a7091ce53620a18a1d3969e19c34e72.496f08b5c5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T06:51:46Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0fbeb1f976399505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.5470c41733a8c8b26caaea6b8c5ec6d96b642274b0003faf3cd8d8a30e1a238e.03ebd74590^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -455,13 +455,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:09:45Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e13d7f4264226f65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.428aae1f954c99f78bcaa6e96df2346772ac82bc464375c14e14c73c5f71a736.c5304e976f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:45:04Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b374e17c2d69f5e7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.a462d25e4b57da4e6d1b9451e2c8d4316c1f0fc30602a0af34984fab9eadcc49.73a3a09814^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT2</t>
@@ -612,10 +612,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T08:12:23Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4c24dd141a8910ef</t>
+    <t xml:space="preserve">2023-07-27T10:04:34Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1e7b57dd5673aefc</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_RAD_KO</t>
@@ -726,10 +726,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T08:29:34Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7165f7e798deca04</t>
+    <t xml:space="preserve">2023-07-27T09:25:09Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e9ada0639943f87d</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
@@ -989,13 +989,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:13:43Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">974b1919c24cb1bc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.bda7ad5255b7d75b1282472305538f05c34754fb65c4f240497c7db88be04e5f.40fe5420b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:47:29Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36001771385a2ebe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.ede287b3e1ea12296fadcf87ab579f82a9b890f2e5593aa19646390d3fe8f636.a08e94eefb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1006,13 +1006,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:15:10Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98f499bce75df3ad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.8b260f9ca1cc69b85c78ed33ff108c32d6777484d26bfac1bca127b29b24dca8.a3229bdea0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:49:49Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8f9c5d410116a799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.a6159ca63ac1dbafb6f7fc2db543448f5751fce7a36457daea64a159a64a20b6.85c80d4e39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [Errore-47| codice fiscale 'PzNMSC00A01F839U' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
@@ -1026,13 +1026,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:20:01Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ef5b3cf9fe31f162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.88f4d6031b3464b82661b6f15004dcfd01d7ad9d80aec2bf751987f836d5ce21.21aecca8e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:53:37Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e1dca066309cb4ad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.7f416bfc3adc6cfad6863818614ed9efb04a0a46aa3a13816394958ae3f15bab.4de9e22c5f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']</t>
@@ -1046,13 +1046,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:21:32Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de51c5f302b8e735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.5e9e5345eb6f694aff99794022388a285a57540dd404ff2f7e88c776ba928f93.d9596e2b42^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:55:21Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d8b1f6a9e731aeb3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.29bd8fa2415d16abb768a91dc528e863e194b63254d0cbc048345b534d7f5dcf.d9987efa8f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
@@ -1066,13 +1066,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:23:30Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deb21fe1426f0855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.c8d730281e108aba64e29d5f3bbe2f3b613ace7d9340a0bcd575de1676951725.3f83a780ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:57:31Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87d35348692fc96d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.312cd23d2d67c865166b7e03ad49455b88ff74a15a297172b3779a7201df2950.8cdbd34905^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
@@ -1086,13 +1086,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:26:18Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38690a86e68007c0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.0b6b75409d951bd1e18d013fff76a451b9eaf8251e98a7a10b2dc318a1a5d278.27e82b0783^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:59:13Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1bf09d66b9541e53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1043a829b12ab047211117bb5c76e36e2238e73a943461e5587861cdd6e40056.0d881f2be5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT11_KO</t>
@@ -1103,13 +1103,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:29:07Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cb0457c05f3278e0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.61597b5b4e967fd8e90f24a898d0ee140ff6defd19f409b72f5f153f3600bf37.5cafb3a68e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T09:03:30Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e228c2844eea8beb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.d6dee5c26324bb9290d1a10a4fd77f18ac7cd089ce5606bdfdbda6ea44adf8c0.9f91cfe326^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ] </t>
@@ -1123,13 +1123,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:31:07Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3c1c15e15fbbef46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.3252c13610be879cc6c8cc5782d49c4885852458a8418aa1d09e389662da92d0.48bb57e3da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T09:05:06Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f77f5c2e83427aca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.d85bc359e53bd2112424fe4c7482d1fd0c58a5f926539f8f53b0a7efdc86ad95.0e9c51b8b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l'elemento 'text']</t>
@@ -1159,13 +1159,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:33:03Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">827d2435f2303d0c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.629cb0ae6ed524c1b5a0b3d412c4e835e62903c1ee5ec73871c0db6cbaf54413.c1617172cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T09:06:44Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8c4007b02456af1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1780b056597ced010448f351f2bcbe3aa01a7b6cc3e3fa8073eb8d02e14dcb58.680b41437b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore vocabolario. Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 78907]</t>
@@ -1457,13 +1457,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-19T13:07:57Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">825a9f113409e0e4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.4d710a8e6f2bc739825998cacf0a40814cad582ce587fabc7c51f0308d65a5ad.4058360a1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">Il software non gestisce  in modo strutturato le informazioni “procedure” richieste dal test case.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -1800,13 +1794,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-07-24T09:06:41Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b631eaa503139c4f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.df142fcbffd7668b3e4038001756f730b1de1b4223e42a244aa287ad67b1f476.e1e7d07502^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-07-27T08:41:51Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ee940bee8ea027a8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.c7e94947b36b06c7b9b46b050dace4e47f26070fd8eaaeef10df145d8e30a085.273a7c3972^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT0</t>
@@ -2545,11 +2539,11 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2632,11 +2626,11 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -2754,15 +2748,15 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="I101" activeCellId="0" sqref="I101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -3161,7 +3155,7 @@
         <v>68</v>
       </c>
       <c r="F13" s="27" t="n">
-        <v>45128</v>
+        <v>45134</v>
       </c>
       <c r="G13" s="28" t="s">
         <v>69</v>
@@ -3249,7 +3243,7 @@
         <v>79</v>
       </c>
       <c r="F15" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G15" s="28" t="s">
         <v>80</v>
@@ -3602,7 +3596,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="100.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="n">
         <v>29</v>
       </c>
@@ -3619,7 +3613,7 @@
         <v>104</v>
       </c>
       <c r="F24" s="34" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G24" s="35" t="s">
         <v>112</v>
@@ -3835,7 +3829,7 @@
         <v>123</v>
       </c>
       <c r="F28" s="34" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G28" s="35" t="s">
         <v>128</v>
@@ -4783,7 +4777,7 @@
         <v>210</v>
       </c>
       <c r="F46" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>211</v>
@@ -4837,7 +4831,7 @@
         <v>215</v>
       </c>
       <c r="F47" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G47" s="28" t="s">
         <v>216</v>
@@ -4891,7 +4885,7 @@
         <v>221</v>
       </c>
       <c r="F48" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G48" s="28" t="s">
         <v>222</v>
@@ -4945,7 +4939,7 @@
         <v>227</v>
       </c>
       <c r="F49" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G49" s="28" t="s">
         <v>228</v>
@@ -4999,7 +4993,7 @@
         <v>233</v>
       </c>
       <c r="F50" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G50" s="28" t="s">
         <v>234</v>
@@ -5053,7 +5047,7 @@
         <v>239</v>
       </c>
       <c r="F51" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G51" s="28" t="s">
         <v>240</v>
@@ -5107,7 +5101,7 @@
         <v>244</v>
       </c>
       <c r="F52" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G52" s="28" t="s">
         <v>245</v>
@@ -5161,7 +5155,7 @@
         <v>250</v>
       </c>
       <c r="F53" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G53" s="28" t="s">
         <v>251</v>
@@ -5291,7 +5285,7 @@
         <v>260</v>
       </c>
       <c r="F56" s="27" t="n">
-        <v>45131</v>
+        <v>45134</v>
       </c>
       <c r="G56" s="28" t="s">
         <v>261</v>
@@ -6280,22 +6274,16 @@
       <c r="E77" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="F77" s="27" t="n">
-        <v>45126</v>
-      </c>
-      <c r="G77" s="28" t="s">
+      <c r="F77" s="27"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="28"/>
+      <c r="I77" s="28"/>
+      <c r="J77" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="K77" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="H77" s="28" t="s">
-        <v>349</v>
-      </c>
-      <c r="I77" s="28" t="s">
-        <v>350</v>
-      </c>
-      <c r="J77" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="K77" s="29"/>
       <c r="L77" s="29"/>
       <c r="M77" s="29"/>
       <c r="N77" s="29"/>
@@ -6319,10 +6307,10 @@
         <v>117</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="28"/>
@@ -6357,10 +6345,10 @@
         <v>117</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F79" s="27"/>
       <c r="G79" s="28"/>
@@ -6395,10 +6383,10 @@
         <v>117</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F80" s="27"/>
       <c r="G80" s="28"/>
@@ -6433,22 +6421,22 @@
         <v>117</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F81" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G81" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="H81" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="I81" s="28" t="s">
         <v>359</v>
-      </c>
-      <c r="H81" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="I81" s="28" t="s">
-        <v>361</v>
       </c>
       <c r="J81" s="29" t="s">
         <v>55</v>
@@ -6487,22 +6475,22 @@
         <v>117</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F82" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G82" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="H82" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="I82" s="28" t="s">
         <v>364</v>
-      </c>
-      <c r="H82" s="28" t="s">
-        <v>365</v>
-      </c>
-      <c r="I82" s="28" t="s">
-        <v>366</v>
       </c>
       <c r="J82" s="29" t="s">
         <v>55</v>
@@ -6515,7 +6503,7 @@
         <v>55</v>
       </c>
       <c r="N82" s="29" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O82" s="29" t="s">
         <v>85</v>
@@ -6541,22 +6529,22 @@
         <v>117</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F83" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G83" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="H83" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="I83" s="28" t="s">
         <v>370</v>
-      </c>
-      <c r="H83" s="28" t="s">
-        <v>371</v>
-      </c>
-      <c r="I83" s="28" t="s">
-        <v>372</v>
       </c>
       <c r="J83" s="29" t="s">
         <v>55</v>
@@ -6569,7 +6557,7 @@
         <v>55</v>
       </c>
       <c r="N83" s="29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="O83" s="29" t="s">
         <v>85</v>
@@ -6595,22 +6583,22 @@
         <v>117</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F84" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G84" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="H84" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="I84" s="28" t="s">
         <v>376</v>
-      </c>
-      <c r="H84" s="28" t="s">
-        <v>377</v>
-      </c>
-      <c r="I84" s="28" t="s">
-        <v>378</v>
       </c>
       <c r="J84" s="29" t="s">
         <v>55</v>
@@ -6649,22 +6637,22 @@
         <v>117</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F85" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G85" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="H85" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="I85" s="28" t="s">
         <v>381</v>
-      </c>
-      <c r="H85" s="28" t="s">
-        <v>382</v>
-      </c>
-      <c r="I85" s="28" t="s">
-        <v>383</v>
       </c>
       <c r="J85" s="29" t="s">
         <v>55</v>
@@ -6703,22 +6691,22 @@
         <v>117</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F86" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G86" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="H86" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="I86" s="28" t="s">
         <v>386</v>
-      </c>
-      <c r="H86" s="28" t="s">
-        <v>387</v>
-      </c>
-      <c r="I86" s="28" t="s">
-        <v>388</v>
       </c>
       <c r="J86" s="29" t="s">
         <v>55</v>
@@ -6757,22 +6745,22 @@
         <v>117</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F87" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G87" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="H87" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="I87" s="28" t="s">
         <v>391</v>
-      </c>
-      <c r="H87" s="28" t="s">
-        <v>392</v>
-      </c>
-      <c r="I87" s="28" t="s">
-        <v>393</v>
       </c>
       <c r="J87" s="29" t="s">
         <v>55</v>
@@ -6785,7 +6773,7 @@
         <v>55</v>
       </c>
       <c r="N87" s="29" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O87" s="29" t="s">
         <v>85</v>
@@ -6811,22 +6799,22 @@
         <v>117</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F88" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G88" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="H88" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="I88" s="28" t="s">
         <v>397</v>
-      </c>
-      <c r="H88" s="28" t="s">
-        <v>398</v>
-      </c>
-      <c r="I88" s="28" t="s">
-        <v>399</v>
       </c>
       <c r="J88" s="29" t="s">
         <v>55</v>
@@ -6839,7 +6827,7 @@
         <v>55</v>
       </c>
       <c r="N88" s="29" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="O88" s="29" t="s">
         <v>85</v>
@@ -6865,22 +6853,22 @@
         <v>117</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F89" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G89" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="H89" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="I89" s="28" t="s">
         <v>403</v>
-      </c>
-      <c r="H89" s="28" t="s">
-        <v>404</v>
-      </c>
-      <c r="I89" s="28" t="s">
-        <v>405</v>
       </c>
       <c r="J89" s="29" t="s">
         <v>55</v>
@@ -6893,7 +6881,7 @@
         <v>55</v>
       </c>
       <c r="N89" s="29" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="O89" s="29" t="s">
         <v>85</v>
@@ -6919,22 +6907,22 @@
         <v>117</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F90" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G90" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="H90" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="I90" s="28" t="s">
         <v>409</v>
-      </c>
-      <c r="H90" s="28" t="s">
-        <v>410</v>
-      </c>
-      <c r="I90" s="28" t="s">
-        <v>411</v>
       </c>
       <c r="J90" s="29" t="s">
         <v>55</v>
@@ -6947,7 +6935,7 @@
         <v>55</v>
       </c>
       <c r="N90" s="29" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="O90" s="29" t="s">
         <v>85</v>
@@ -6973,22 +6961,22 @@
         <v>117</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F91" s="27" t="n">
         <v>45127</v>
       </c>
       <c r="G91" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="H91" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="I91" s="28" t="s">
         <v>415</v>
-      </c>
-      <c r="H91" s="28" t="s">
-        <v>416</v>
-      </c>
-      <c r="I91" s="28" t="s">
-        <v>417</v>
       </c>
       <c r="J91" s="29" t="s">
         <v>55</v>
@@ -7001,7 +6989,7 @@
         <v>55</v>
       </c>
       <c r="N91" s="29" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="O91" s="29" t="s">
         <v>85</v>
@@ -7027,10 +7015,10 @@
         <v>117</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F92" s="27"/>
       <c r="G92" s="28"/>
@@ -7065,10 +7053,10 @@
         <v>117</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E93" s="26" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F93" s="27"/>
       <c r="G93" s="28"/>
@@ -7103,10 +7091,10 @@
         <v>117</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E94" s="26" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F94" s="27"/>
       <c r="G94" s="28"/>
@@ -7141,10 +7129,10 @@
         <v>117</v>
       </c>
       <c r="D95" s="25" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F95" s="27"/>
       <c r="G95" s="28"/>
@@ -7179,10 +7167,10 @@
         <v>117</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F96" s="27"/>
       <c r="G96" s="28"/>
@@ -7217,10 +7205,10 @@
         <v>117</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F97" s="27"/>
       <c r="G97" s="28"/>
@@ -7255,10 +7243,10 @@
         <v>117</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E98" s="26" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F98" s="27"/>
       <c r="G98" s="28"/>
@@ -7293,22 +7281,22 @@
         <v>117</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E99" s="26" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F99" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G99" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="H99" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="I99" s="28" t="s">
         <v>435</v>
-      </c>
-      <c r="H99" s="28" t="s">
-        <v>436</v>
-      </c>
-      <c r="I99" s="28" t="s">
-        <v>437</v>
       </c>
       <c r="J99" s="29" t="s">
         <v>55</v>
@@ -7321,7 +7309,7 @@
         <v>55</v>
       </c>
       <c r="N99" s="29" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="O99" s="29" t="s">
         <v>85</v>
@@ -7347,22 +7335,22 @@
         <v>49</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E100" s="26" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F100" s="27" t="n">
         <v>45128</v>
       </c>
       <c r="G100" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="H100" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="I100" s="28" t="s">
         <v>441</v>
-      </c>
-      <c r="H100" s="28" t="s">
-        <v>442</v>
-      </c>
-      <c r="I100" s="28" t="s">
-        <v>443</v>
       </c>
       <c r="J100" s="29" t="s">
         <v>55</v>
@@ -7380,7 +7368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="100.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="24" t="n">
         <v>369</v>
       </c>
@@ -7391,22 +7379,22 @@
         <v>77</v>
       </c>
       <c r="D101" s="25" t="s">
+        <v>442</v>
+      </c>
+      <c r="E101" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="F101" s="27" t="n">
+        <v>45134</v>
+      </c>
+      <c r="G101" s="28" t="s">
         <v>444</v>
       </c>
-      <c r="E101" s="26" t="s">
+      <c r="H101" s="28" t="s">
         <v>445</v>
       </c>
-      <c r="F101" s="27" t="n">
-        <v>45131</v>
-      </c>
-      <c r="G101" s="28" t="s">
+      <c r="I101" s="28" t="s">
         <v>446</v>
-      </c>
-      <c r="H101" s="28" t="s">
-        <v>447</v>
-      </c>
-      <c r="I101" s="28" t="s">
-        <v>448</v>
       </c>
       <c r="J101" s="29" t="s">
         <v>55</v>
@@ -7435,22 +7423,22 @@
         <v>91</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E102" s="26" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F102" s="27" t="n">
         <v>45127</v>
       </c>
       <c r="G102" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="H102" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="I102" s="28" t="s">
         <v>451</v>
-      </c>
-      <c r="H102" s="28" t="s">
-        <v>452</v>
-      </c>
-      <c r="I102" s="28" t="s">
-        <v>453</v>
       </c>
       <c r="J102" s="29" t="s">
         <v>55</v>
@@ -7479,22 +7467,22 @@
         <v>117</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F103" s="27" t="n">
         <v>45126</v>
       </c>
       <c r="G103" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="H103" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="I103" s="28" t="s">
         <v>456</v>
-      </c>
-      <c r="H103" s="28" t="s">
-        <v>457</v>
-      </c>
-      <c r="I103" s="28" t="s">
-        <v>458</v>
       </c>
       <c r="J103" s="29" t="s">
         <v>55</v>
@@ -12483,13 +12471,13 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -12506,10 +12494,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12517,13 +12505,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>460</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>461</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>462</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12531,13 +12519,13 @@
         <v>77</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12545,55 +12533,55 @@
         <v>91</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="37" t="s">
         <v>468</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>469</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>471</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>472</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>473</v>
+      </c>
+      <c r="D7" s="38" t="s">
         <v>474</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>475</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12601,41 +12589,41 @@
         <v>117</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
+        <v>477</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="D9" s="38" t="s">
         <v>479</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>480</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>481</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>482</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12643,13 +12631,13 @@
         <v>49</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C11" s="37" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12657,13 +12645,13 @@
         <v>77</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C12" s="37" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12671,55 +12659,55 @@
         <v>91</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C13" s="37" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C14" s="37" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C15" s="37" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C16" s="37" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12727,27 +12715,27 @@
         <v>117</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C17" s="37" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C18" s="37" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12755,13 +12743,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C19" s="37" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12769,13 +12757,13 @@
         <v>77</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C20" s="37" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12783,55 +12771,55 @@
         <v>91</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C21" s="37" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C22" s="37" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C23" s="37" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C24" s="37" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12839,27 +12827,27 @@
         <v>117</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C25" s="37" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C26" s="37" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12867,13 +12855,13 @@
         <v>49</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C27" s="37" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12881,13 +12869,13 @@
         <v>77</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C28" s="37" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12895,55 +12883,55 @@
         <v>91</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C29" s="37" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C30" s="37" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C31" s="37" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C32" s="37" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12951,27 +12939,27 @@
         <v>117</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C33" s="37" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C34" s="37" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12979,7 +12967,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C35" s="37" t="n">
         <v>195</v>
@@ -12993,7 +12981,7 @@
         <v>77</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C36" s="37" t="n">
         <v>211</v>
@@ -13007,7 +12995,7 @@
         <v>91</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C37" s="37" t="n">
         <v>227</v>
@@ -13018,10 +13006,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C38" s="37" t="n">
         <v>243</v>
@@ -13032,10 +13020,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C39" s="37" t="n">
         <v>259</v>
@@ -13046,10 +13034,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C40" s="37" t="n">
         <v>275</v>
@@ -13063,7 +13051,7 @@
         <v>117</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C41" s="37" t="n">
         <v>291</v>
@@ -13074,10 +13062,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C42" s="37" t="n">
         <v>307</v>
@@ -13091,7 +13079,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C43" s="37" t="n">
         <v>196</v>
@@ -13105,7 +13093,7 @@
         <v>77</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C44" s="37" t="n">
         <v>212</v>
@@ -13119,7 +13107,7 @@
         <v>91</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C45" s="37" t="n">
         <v>228</v>
@@ -13130,10 +13118,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C46" s="37" t="n">
         <v>244</v>
@@ -13144,10 +13132,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C47" s="37" t="n">
         <v>260</v>
@@ -13158,10 +13146,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C48" s="37" t="n">
         <v>276</v>
@@ -13175,7 +13163,7 @@
         <v>117</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C49" s="37" t="n">
         <v>292</v>
@@ -13186,10 +13174,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C50" s="37" t="n">
         <v>308</v>
@@ -14166,11 +14154,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -14187,7 +14175,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="40" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B2" s="40" t="s">
         <v>55</v>
@@ -14195,7 +14183,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B3" s="40" t="s">
         <v>85</v>

</xml_diff>